<commit_message>
Modify time integation for power profile
</commit_message>
<xml_diff>
--- a/tests/input_data/trey_data.xlsx
+++ b/tests/input_data/trey_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\lutomasini\git\pandapower-heig-ui\.cache\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lutomasini\git\pandapower-heig-ui\tests\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426F8B3-476B-41C9-B889-ADACB707FE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7CFD7E-9100-4767-B6D6-F39F838224A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D466C24-507B-41DF-96AE-5E0A3D434556}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1922,7 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove vector group madatory
</commit_message>
<xml_diff>
--- a/tests/input_data/trey_data.xlsx
+++ b/tests/input_data/trey_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lutomasini\git\pandapower-heig-ui\tests\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thierryfra\github\pro\pandapower-heig-ui\tests\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7CFD7E-9100-4767-B6D6-F39F838224A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A843150A-5F7B-46C7-BAE4-A9E1F71A7DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
   <si>
     <t>name</t>
   </si>
@@ -310,9 +310,6 @@
   </si>
   <si>
     <t>trafo_0</t>
-  </si>
-  <si>
-    <t>Dyn</t>
   </si>
   <si>
     <t>lv</t>
@@ -465,15 +462,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -506,9 +502,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -546,7 +542,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -652,7 +648,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -794,7 +790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -808,19 +804,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D1" t="s">
@@ -833,12 +829,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2">
         <v>18</v>
@@ -847,12 +843,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>0.4</v>
@@ -861,12 +857,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>0.4</v>
@@ -875,12 +871,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>0.4</v>
@@ -889,12 +885,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>0.4</v>
@@ -903,12 +899,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -917,12 +913,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8">
         <v>0.4</v>
@@ -931,12 +927,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>0.4</v>
@@ -945,12 +941,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10">
         <v>0.4</v>
@@ -959,12 +955,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <v>0.4</v>
@@ -973,12 +969,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>0.4</v>
@@ -987,12 +983,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13">
         <v>0.4</v>
@@ -1001,12 +997,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14">
         <v>0.4</v>
@@ -1015,92 +1011,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1115,46 +1111,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D466C24-507B-41DF-96AE-5E0A3D434556}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>36</v>
       </c>
       <c r="J1" t="s">
@@ -1163,13 +1159,13 @@
       <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>40</v>
       </c>
       <c r="O1" t="s">
@@ -1185,11 +1181,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C2">
@@ -1223,11 +1219,11 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C3">
@@ -1261,11 +1257,11 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C4">
@@ -1289,7 +1285,7 @@
       <c r="I4">
         <v>0.17</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="5"/>
       <c r="L4">
         <v>0.38700000000000001</v>
       </c>
@@ -1300,11 +1296,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C5">
@@ -1328,7 +1324,7 @@
       <c r="I5">
         <v>0.17</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="5"/>
       <c r="L5">
         <v>0.38700000000000001</v>
       </c>
@@ -1339,11 +1335,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C6">
@@ -1377,11 +1373,11 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C7">
@@ -1415,11 +1411,11 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C8">
@@ -1443,7 +1439,7 @@
       <c r="I8">
         <v>0.17</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="5"/>
       <c r="L8">
         <v>0.38700000000000001</v>
       </c>
@@ -1454,11 +1450,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C9">
@@ -1482,7 +1478,7 @@
       <c r="I9">
         <v>0.17</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="5"/>
       <c r="L9">
         <v>0.38700000000000001</v>
       </c>
@@ -1493,11 +1489,11 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C10">
@@ -1531,11 +1527,11 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C11">
@@ -1569,11 +1565,11 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C12">
@@ -1607,102 +1603,102 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1720,28 +1716,28 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G1" t="s">
@@ -1757,157 +1753,157 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1921,70 +1917,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3219A80D-1395-476B-8C71-29B1418CDB59}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" customWidth="1"/>
-    <col min="26" max="26" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="15" max="15" width="14.1796875" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.453125" customWidth="1"/>
+    <col min="24" max="24" width="19.453125" customWidth="1"/>
+    <col min="26" max="26" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="R1" s="2" t="s">
@@ -2014,20 +2010,20 @@
       <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2062,9 +2058,6 @@
       <c r="K2">
         <v>1.9</v>
       </c>
-      <c r="L2" t="s">
-        <v>90</v>
-      </c>
       <c r="M2">
         <v>3</v>
       </c>
@@ -2082,7 +2075,7 @@
         <v>1.9</v>
       </c>
       <c r="S2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -2100,152 +2093,152 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2263,68 +2256,68 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="9"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="8"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>50</v>
       </c>
       <c r="M1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2">
         <v>100</v>
       </c>
@@ -2338,153 +2331,153 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2503,27 +2496,27 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="24" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" customWidth="1"/>
+    <col min="13" max="24" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E1" t="s">
@@ -2536,16 +2529,16 @@
         <v>80</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="L1" t="s">
         <v>87</v>
@@ -2554,12 +2547,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2574,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J2">
         <v>1.2</v>
@@ -2586,12 +2579,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -2606,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3">
         <v>1.2</v>
@@ -2618,12 +2611,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -2638,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J4">
         <v>1.2</v>
@@ -2650,142 +2643,142 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2805,22 +2798,22 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D1" t="s">
@@ -2833,7 +2826,7 @@
         <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
         <v>78</v>
@@ -2841,7 +2834,7 @@
       <c r="I1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
@@ -2851,7 +2844,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2871,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2891,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2911,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2931,7 +2924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2951,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2971,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2991,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3011,7 +3004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3031,7 +3024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3051,7 +3044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3071,7 +3064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3091,97 +3084,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>

</xml_diff>